<commit_message>
q2 earnings call added
</commit_message>
<xml_diff>
--- a/FCX.xlsx
+++ b/FCX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Development\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C038087-7AEC-47D5-88EF-ADA9F5F52638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9F202D-088F-4D39-857E-83E7CE52154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19020" windowHeight="20985" tabRatio="767" activeTab="3" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19020" windowHeight="20985" tabRatio="767" activeTab="5" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="WORKINGS&gt;&gt;" sheetId="9" r:id="rId3"/>
     <sheet name="Historical" sheetId="10" r:id="rId4"/>
     <sheet name="INPUT&gt;&gt;" sheetId="6" r:id="rId5"/>
+    <sheet name="Q2_earnings_call_notes" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
   <si>
     <r>
       <t xml:space="preserve">This Excel file is intended </t>
@@ -398,6 +399,45 @@
   </si>
   <si>
     <t>Gross-margin</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Jun 25</t>
+  </si>
+  <si>
+    <t>Copper is in the focus of the world</t>
+  </si>
+  <si>
+    <t>FCX is the dominant producer in the US (&gt;70% market share)</t>
+  </si>
+  <si>
+    <t>Startup of Indonesian smelter</t>
+  </si>
+  <si>
+    <t>Fully integrated producer globally</t>
+  </si>
+  <si>
+    <t>copper sales will be 10% higher than in first halve year</t>
+  </si>
+  <si>
+    <t>Additional margins and CF</t>
+  </si>
+  <si>
+    <t>Volume growth and lower costs for 2026</t>
+  </si>
+  <si>
+    <t>2.9mn shares were bought back in H1</t>
+  </si>
+  <si>
+    <t>50% of FCF are supposed to be used for share buybacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decreased reliance on contractors </t>
+  </si>
+  <si>
+    <t>till minute 20</t>
   </si>
 </sst>
 </file>
@@ -1379,10 +1419,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:AF750"/>
+  <dimension ref="A1:AF751"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" topLeftCell="J4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -3466,48 +3506,97 @@
       <c r="T40" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="U40" s="17"/>
+      <c r="U40" s="17" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" spans="3:32" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="3:32" x14ac:dyDescent="0.2">
-      <c r="E42" s="2" t="s">
-        <v>22</v>
+      <c r="E42" s="39" t="s">
+        <v>99</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="46"/>
+      <c r="P42" s="46"/>
+      <c r="Q42" s="46">
+        <v>5273</v>
+      </c>
+      <c r="R42" s="46"/>
+      <c r="S42" s="46"/>
+      <c r="T42" s="46"/>
+      <c r="U42" s="46">
+        <v>4490</v>
+      </c>
     </row>
     <row r="43" spans="3:32" x14ac:dyDescent="0.2">
-      <c r="E43" s="10" t="s">
-        <v>49</v>
+      <c r="E43" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="46"/>
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
     </row>
     <row r="44" spans="3:32" x14ac:dyDescent="0.2">
       <c r="E44" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
+      <c r="N44" s="46"/>
+      <c r="O44" s="46"/>
+      <c r="P44" s="46"/>
+      <c r="Q44" s="46"/>
+      <c r="R44" s="46"/>
+      <c r="S44" s="46"/>
+      <c r="T44" s="46"/>
+      <c r="U44" s="46"/>
     </row>
     <row r="45" spans="3:32" x14ac:dyDescent="0.2">
-      <c r="E45" s="9"/>
+      <c r="E45" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
+      <c r="N45" s="46"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="46"/>
+      <c r="T45" s="46"/>
+      <c r="U45" s="46"/>
     </row>
     <row r="46" spans="3:32" x14ac:dyDescent="0.2">
+      <c r="E46" s="9"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -3515,32 +3604,15 @@
       <c r="J46" s="12"/>
     </row>
     <row r="47" spans="3:32" x14ac:dyDescent="0.2">
-      <c r="E47" s="4" t="s">
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+    </row>
+    <row r="48" spans="3:32" x14ac:dyDescent="0.2">
+      <c r="E48" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-    </row>
-    <row r="48" spans="3:32" x14ac:dyDescent="0.2">
-      <c r="C48" s="11" t="b" cm="1">
-        <f t="array" ref="C48">AND(F48:J48&lt;$B$1,F48:J48&gt;-$B$1)</f>
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
@@ -3558,208 +3630,227 @@
       <c r="T48" s="15"/>
       <c r="U48" s="15"/>
     </row>
-    <row r="49" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-    </row>
-    <row r="50" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E50" s="2" t="str">
+    <row r="49" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C49" s="11" t="b" cm="1">
+        <f t="array" ref="C49">AND(F49:J49&lt;$B$1,F49:J49&gt;-$B$1)</f>
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+    </row>
+    <row r="50" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="E51" s="2" t="str">
         <f>Input!$E$8&amp;" - CF"</f>
         <v>FCX - CF</v>
       </c>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E51" s="6" t="str">
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="E52" s="6" t="str">
         <f>+Input!$E$14</f>
         <v>$mn</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F52" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G51" s="17" t="s">
+      <c r="G52" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H51" s="17" t="s">
+      <c r="H52" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I51" s="17" t="s">
+      <c r="I52" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J52" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L51" s="17" t="s">
+      <c r="L52" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M51" s="17" t="s">
+      <c r="M52" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N51" s="17" t="s">
+      <c r="N52" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="O51" s="17" t="s">
+      <c r="O52" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="P51" s="17" t="s">
+      <c r="P52" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="Q51" s="17" t="s">
+      <c r="Q52" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="R51" s="17" t="s">
+      <c r="R52" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="S51" s="17" t="s">
+      <c r="S52" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="T51" s="17" t="s">
+      <c r="T52" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="U51" s="17"/>
-    </row>
-    <row r="52" spans="5:21" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E53" s="9" t="s">
+      <c r="U52" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="3:21" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="E54" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-    </row>
-    <row r="54" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E54" s="9" t="s">
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="E55" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="14"/>
-      <c r="U54" s="35"/>
-    </row>
-    <row r="55" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="35"/>
+    </row>
+    <row r="56" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="E56" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="13">
-        <f t="shared" ref="F55:I55" si="31">+F53+F54</f>
+      <c r="F56" s="13">
+        <f t="shared" ref="F56:I56" si="31">+F54+F55</f>
         <v>0</v>
       </c>
-      <c r="G55" s="13">
+      <c r="G56" s="13">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="H55" s="13">
+      <c r="H56" s="13">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="I55" s="13">
+      <c r="I56" s="13">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="J55" s="13">
-        <f>+J53+J54</f>
+      <c r="J56" s="13">
+        <f>+J54+J55</f>
         <v>0</v>
       </c>
-      <c r="L55" s="13">
-        <f t="shared" ref="L55:T55" si="32">+L53+L54</f>
+      <c r="L56" s="13">
+        <f t="shared" ref="L56:T56" si="32">+L54+L55</f>
         <v>0</v>
       </c>
-      <c r="M55" s="13">
+      <c r="M56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="N55" s="13">
+      <c r="N56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="O55" s="13">
+      <c r="O56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="P55" s="13">
+      <c r="P56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="Q55" s="13">
+      <c r="Q56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="R55" s="13">
+      <c r="R56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="S55" s="13">
+      <c r="S56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="T55" s="13">
+      <c r="T56" s="13">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="U55" s="13"/>
-    </row>
-    <row r="56" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E56" s="9" t="s">
+      <c r="U56" s="13"/>
+    </row>
+    <row r="57" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="E57" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-    </row>
-    <row r="59" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-    </row>
-    <row r="60" spans="5:21" x14ac:dyDescent="0.2">
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+    </row>
+    <row r="60" spans="3:21" x14ac:dyDescent="0.2">
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
     </row>
-    <row r="61" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:21" x14ac:dyDescent="0.2">
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
     </row>
-    <row r="62" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:21" x14ac:dyDescent="0.2">
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
     </row>
-    <row r="63" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:21" x14ac:dyDescent="0.2">
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
     </row>
-    <row r="64" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:21" x14ac:dyDescent="0.2">
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -8567,6 +8658,13 @@
       <c r="H750" s="12"/>
       <c r="I750" s="12"/>
       <c r="J750" s="12"/>
+    </row>
+    <row r="751" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F751" s="12"/>
+      <c r="G751" s="12"/>
+      <c r="H751" s="12"/>
+      <c r="I751" s="12"/>
+      <c r="J751" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
@@ -8579,7 +8677,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
+  <conditionalFormatting sqref="C49">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -8602,4 +8700,74 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628ACCA-55C0-49BE-B8AF-DF2B2BD6A718}">
+  <dimension ref="C5:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>